<commit_message>
added a doc about mutual scoring
</commit_message>
<xml_diff>
--- a/Admin/2015-TH-XLP-流程及计分规则 1.26  21：25.xlsx
+++ b/Admin/2015-TH-XLP-流程及计分规则 1.26  21：25.xlsx
@@ -1377,39 +1377,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>讨论过程中必须使用罗伯特议事规则，635书面头
-脑风暴模版和商业模式画布三种工具中一到三种。。（5分）
-讨论过程中各成员参与度、发言质量。（3分）
-每个小组都必须持有会议展开的记录（文字，相片，视频）
-等并且上传至git各小组项目中</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">    命名为第三次会议                        </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="2"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>截至时间为11：00（20分）</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>文档要求：必须至少分工四组                                      （即原组成员不变，但可以通过交易形成暂时的雇佣关系，被雇佣者仍隶属与原组，但需在任务分工文档中注明）                                                          各组专做宪章、微电影、网页、实物其中之一
 关于筹备组工作，                                              由项目经理决定其是否专干（不再参与原组的工作），
 若专干，则也需要在文档中说明和备注筹备组与全组成员之间的协议</t>
@@ -1962,6 +1929,39 @@
   </si>
   <si>
     <r>
+      <t>讨论过程中必须使用罗伯特议事规则，635书面头
+脑风暴模版和商业模式画布三种工具中一到三种。。（5分）
+讨论过程中各成员参与度、发言质量。（3分）
+每个小组都必须持有会议展开的记录（文字，相片，视频）
+等并且上传至git各小组项目中</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">    命名为第三次会议                        </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>截至时间为11：00（20分）</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
       <t>各组所有成员必须统一参与一次整组讨论，进行分工
 讨论过程中必须使用罗伯特议事规则，635书面头
 脑风暴模版和商业模式画布三种工具中一到三种。（5分）
@@ -2016,7 +2016,7 @@
       </rPr>
       <t xml:space="preserve">
 截止日期为2015年1月29日10：50。延时上交者取消展示资格
-各小组在合并前需要将自己组的成果都确定下来.截止日期为1月29日14:00
+各小组在合并前需要将自己组的成果都确定下来.截止日期为1月29日12:00
 在此时间之后的修改不会被计入第一次git的100分记分组评分
 </t>
     </r>
@@ -2962,10 +2962,10 @@
   <dimension ref="A1:EI51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="H29" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3311,7 +3311,7 @@
         <v>28</v>
       </c>
       <c r="I13" s="40" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="J13" s="46" t="s">
         <v>193</v>
@@ -3390,7 +3390,7 @@
       <c r="H16" s="39"/>
       <c r="I16" s="40"/>
       <c r="J16" s="55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="119.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3420,7 +3420,7 @@
         <v>189</v>
       </c>
       <c r="J17" s="57" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="182.1" customHeight="1" x14ac:dyDescent="0.15">
@@ -3447,7 +3447,7 @@
         <v>28</v>
       </c>
       <c r="I18" s="40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J18" s="56"/>
     </row>
@@ -3503,7 +3503,7 @@
         <v>5</v>
       </c>
       <c r="I20" s="40" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="J20" s="41" t="s">
         <v>174</v>
@@ -3616,7 +3616,7 @@
         <v>108</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G25" s="38" t="s">
         <v>118</v>
@@ -3651,7 +3651,7 @@
         <v>13</v>
       </c>
       <c r="I26" s="40" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="J26" s="41" t="s">
         <v>195</v>
@@ -3777,7 +3777,7 @@
         <v>28</v>
       </c>
       <c r="I31" s="40" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J31" s="41"/>
     </row>
@@ -3803,7 +3803,7 @@
         <v>5</v>
       </c>
       <c r="I32" s="40" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="J32" s="41" t="s">
         <v>170</v>
@@ -4054,10 +4054,10 @@
         <v>30</v>
       </c>
       <c r="I37" s="40" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="J37" s="41" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="38" spans="1:139" s="5" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.15">
@@ -4156,7 +4156,7 @@
         <v>5</v>
       </c>
       <c r="I41" s="40" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="J41" s="41"/>
     </row>

</xml_diff>